<commit_message>
manually selected the videos for each year
</commit_message>
<xml_diff>
--- a/data/df_videos_2017.xlsx
+++ b/data/df_videos_2017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzobehna/projects/Social-Computing_Final-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F58D5E40-320C-BB48-979F-977219B04E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58E6C1D-AEA4-284C-9D43-4D3BC8B0C26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{60A97FFF-FF88-914B-8116-3CE092488C52}"/>
   </bookViews>
@@ -873,7 +873,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1056,6 +1056,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1220,15 +1226,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1607,10 +1608,13 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:J21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="120.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1666,7 +1670,7 @@
       <c r="G2">
         <v>23100</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
       <c r="I2" t="s">
@@ -1698,7 +1702,7 @@
       <c r="G3">
         <v>7257</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
       <c r="I3" t="s">
@@ -1730,7 +1734,7 @@
       <c r="G4">
         <v>30411</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>29</v>
       </c>
       <c r="I4" t="s">
@@ -1762,7 +1766,7 @@
       <c r="G5">
         <v>22915</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>36</v>
       </c>
       <c r="I5" t="s">
@@ -1794,7 +1798,7 @@
       <c r="G6">
         <v>7660</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>43</v>
       </c>
       <c r="I6" t="s">
@@ -1826,7 +1830,7 @@
       <c r="G7">
         <v>12446</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>50</v>
       </c>
       <c r="I7" t="s">
@@ -1922,7 +1926,7 @@
       <c r="G10">
         <v>2376</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>69</v>
       </c>
       <c r="I10" t="s">
@@ -1954,7 +1958,7 @@
       <c r="G11" s="2">
         <v>4256</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1968,325 +1972,325 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>1837879</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>1145</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>1791861</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>8056</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>27</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>1677573</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>4868</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>1079563</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>1279</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>812627</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>2039</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>673781</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>908</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="e">
+      <c r="A18" s="1" t="e">
         <v>#NAME?</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>596153</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>1189</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>579430</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>575</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>514238</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>566</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>511161</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>1425</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
         <v>25</v>
       </c>
     </row>

</xml_diff>